<commit_message>
Grades input changed to checkbox and working properly
</commit_message>
<xml_diff>
--- a/Herramienta/static/files/ExportarActividad.xlsx
+++ b/Herramienta/static/files/ExportarActividad.xlsx
@@ -20,7 +20,7 @@
     <t>Nombre:</t>
   </si>
   <si>
-    <t>2014-10 Prueba</t>
+    <t>2014-10 Prueba 2</t>
   </si>
   <si>
     <t>Semestre:</t>
@@ -89,7 +89,7 @@
     <t>Penalización por entregar tarde el informe</t>
   </si>
   <si>
-    <t>1. Burger Xpress</t>
+    <t>Burger Xpress</t>
   </si>
   <si>
     <t>a. Formulación General</t>
@@ -266,7 +266,7 @@
     <t>Los resultados no se presentan</t>
   </si>
   <si>
-    <t>2. Método Gráfico</t>
+    <t>Método Gráfico</t>
   </si>
   <si>
     <t>a. Formulación Explícita</t>
@@ -677,7 +677,7 @@
     <t>No hace comentarios o los hace de forma incorrecta</t>
   </si>
   <si>
-    <t>4. Selección de Proyectos</t>
+    <t>Selección de Proyectos</t>
   </si>
   <si>
     <t>Se debe invertir solo una vez en cada proyecto</t>
@@ -800,7 +800,7 @@
     <t>d. Implementación en Xpress-MP</t>
   </si>
   <si>
-    <t>5. Bono 1</t>
+    <t>Bono 1</t>
   </si>
   <si>
     <t>Formulación e Implementación</t>
@@ -1395,7 +1395,7 @@
         <v>29</v>
       </c>
       <c r="H23" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I23" t="n">
         <v>1</v>
@@ -1465,7 +1465,7 @@
         <v>34</v>
       </c>
       <c r="H28" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I28" t="n">
         <v>1</v>
@@ -1521,7 +1521,7 @@
         <v>38</v>
       </c>
       <c r="H32" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="I32" t="n">
         <v>1</v>
@@ -1535,7 +1535,7 @@
         <v>39</v>
       </c>
       <c r="H33" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="I33" t="n">
         <v>1</v>
@@ -1599,7 +1599,7 @@
         <v>44</v>
       </c>
       <c r="H38" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="I38" t="n">
         <v>1</v>
@@ -1655,7 +1655,7 @@
         <v>44</v>
       </c>
       <c r="H42" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="I42" t="n">
         <v>1</v>
@@ -1781,7 +1781,7 @@
         <v>53</v>
       </c>
       <c r="H51" t="n">
-        <v>1</v>
+        <v>1.8</v>
       </c>
       <c r="I51" t="n">
         <v>1</v>
@@ -1851,7 +1851,7 @@
         <v>55</v>
       </c>
       <c r="H56" t="n">
-        <v>1</v>
+        <v>1.8</v>
       </c>
       <c r="I56" t="n">
         <v>1</v>
@@ -1949,7 +1949,7 @@
         <v>49</v>
       </c>
       <c r="H63" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="I63" t="n">
         <v>1</v>
@@ -2005,7 +2005,7 @@
         <v>62</v>
       </c>
       <c r="H67" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I67" t="n">
         <v>1</v>
@@ -2069,7 +2069,7 @@
         <v>66</v>
       </c>
       <c r="H72" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="I72" t="n">
         <v>1</v>
@@ -2141,7 +2141,7 @@
         <v>72</v>
       </c>
       <c r="H78" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="I78" t="n">
         <v>1</v>
@@ -2267,7 +2267,7 @@
         <v>81</v>
       </c>
       <c r="H87" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="I87" t="n">
         <v>1</v>
@@ -2350,7 +2350,7 @@
         <v>0</v>
       </c>
       <c r="H94" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="95" spans="1:9">
@@ -2361,7 +2361,7 @@
         <v>87</v>
       </c>
       <c r="H95" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I95" t="n">
         <v>1</v>
@@ -2375,7 +2375,7 @@
         <v>39</v>
       </c>
       <c r="H96" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I96" t="n">
         <v>1</v>
@@ -2439,7 +2439,7 @@
         <v>91</v>
       </c>
       <c r="H101" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I101" t="n">
         <v>1</v>
@@ -2470,7 +2470,7 @@
         <v>0</v>
       </c>
       <c r="H103" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="104" spans="1:9">
@@ -2481,7 +2481,7 @@
         <v>94</v>
       </c>
       <c r="H104" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I104" t="n">
         <v>1</v>
@@ -2495,7 +2495,7 @@
         <v>95</v>
       </c>
       <c r="H105" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I105" t="n">
         <v>1</v>
@@ -2526,7 +2526,7 @@
         <v>0</v>
       </c>
       <c r="H107" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="108" spans="1:9">
@@ -2537,7 +2537,7 @@
         <v>97</v>
       </c>
       <c r="H108" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I108" t="n">
         <v>1</v>
@@ -2568,7 +2568,7 @@
         <v>0</v>
       </c>
       <c r="H110" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="111" spans="1:9">
@@ -2579,7 +2579,7 @@
         <v>99</v>
       </c>
       <c r="H111" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I111" t="n">
         <v>1</v>
@@ -2643,7 +2643,7 @@
         <v>103</v>
       </c>
       <c r="H116" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I116" t="n">
         <v>1</v>
@@ -2768,7 +2768,7 @@
         <v>0</v>
       </c>
       <c r="H126" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="127" spans="1:9">
@@ -2779,7 +2779,7 @@
         <v>114</v>
       </c>
       <c r="H127" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I127" t="n">
         <v>1</v>
@@ -2810,7 +2810,7 @@
         <v>0</v>
       </c>
       <c r="H129" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="130" spans="1:9">
@@ -2821,7 +2821,7 @@
         <v>117</v>
       </c>
       <c r="H130" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I130" t="n">
         <v>1</v>
@@ -2893,7 +2893,7 @@
         <v>122</v>
       </c>
       <c r="H136" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="I136" t="n">
         <v>1</v>
@@ -2963,7 +2963,7 @@
         <v>126</v>
       </c>
       <c r="H141" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I141" t="n">
         <v>1</v>
@@ -2977,7 +2977,7 @@
         <v>127</v>
       </c>
       <c r="H142" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="I142" t="n">
         <v>1</v>
@@ -3005,7 +3005,7 @@
         <v>129</v>
       </c>
       <c r="H144" t="n">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="I144" t="n">
         <v>1</v>
@@ -3121,7 +3121,7 @@
         <v>138</v>
       </c>
       <c r="H154" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I154" t="n">
         <v>1</v>
@@ -3166,7 +3166,7 @@
         <v>0</v>
       </c>
       <c r="H157" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="158" spans="1:9">
@@ -3177,7 +3177,7 @@
         <v>142</v>
       </c>
       <c r="H158" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I158" t="n">
         <v>1</v>
@@ -3208,7 +3208,7 @@
         <v>0</v>
       </c>
       <c r="H160" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="161" spans="1:9">
@@ -3219,7 +3219,7 @@
         <v>145</v>
       </c>
       <c r="H161" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I161" t="n">
         <v>1</v>
@@ -3250,7 +3250,7 @@
         <v>0</v>
       </c>
       <c r="H163" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="164" spans="1:9">
@@ -3261,7 +3261,7 @@
         <v>148</v>
       </c>
       <c r="H164" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I164" t="n">
         <v>1</v>
@@ -3300,7 +3300,7 @@
         <v>0</v>
       </c>
       <c r="H167" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="168" spans="1:9">
@@ -3311,7 +3311,7 @@
         <v>150</v>
       </c>
       <c r="H168" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="I168" t="n">
         <v>1</v>
@@ -3325,7 +3325,7 @@
         <v>151</v>
       </c>
       <c r="H169" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I169" t="n">
         <v>1</v>
@@ -3370,7 +3370,7 @@
         <v>0</v>
       </c>
       <c r="H172" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="173" spans="1:9">
@@ -3381,7 +3381,7 @@
         <v>154</v>
       </c>
       <c r="H173" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I173" t="n">
         <v>1</v>
@@ -3428,7 +3428,7 @@
         <v>0</v>
       </c>
       <c r="H177" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="178" spans="1:9">
@@ -3439,7 +3439,7 @@
         <v>137</v>
       </c>
       <c r="H178" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I178" t="n">
         <v>1</v>
@@ -3498,7 +3498,7 @@
         <v>0</v>
       </c>
       <c r="H182" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="183" spans="1:9">
@@ -3509,7 +3509,7 @@
         <v>158</v>
       </c>
       <c r="H183" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="I183" t="n">
         <v>1</v>
@@ -3540,7 +3540,7 @@
         <v>0</v>
       </c>
       <c r="H185" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="186" spans="1:9">
@@ -3551,7 +3551,7 @@
         <v>159</v>
       </c>
       <c r="H186" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I186" t="n">
         <v>1</v>
@@ -3582,7 +3582,7 @@
         <v>0</v>
       </c>
       <c r="H188" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="189" spans="1:9">
@@ -3593,7 +3593,7 @@
         <v>148</v>
       </c>
       <c r="H189" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I189" t="n">
         <v>1</v>
@@ -3632,7 +3632,7 @@
         <v>0</v>
       </c>
       <c r="H192" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="193" spans="1:9">
@@ -3643,7 +3643,7 @@
         <v>160</v>
       </c>
       <c r="H193" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I193" t="n">
         <v>1</v>
@@ -3657,7 +3657,7 @@
         <v>161</v>
       </c>
       <c r="H194" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="I194" t="n">
         <v>1</v>
@@ -3718,7 +3718,7 @@
         <v>0</v>
       </c>
       <c r="H199" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="200" spans="1:9">
@@ -3729,7 +3729,7 @@
         <v>137</v>
       </c>
       <c r="H200" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I200" t="n">
         <v>1</v>
@@ -3788,7 +3788,7 @@
         <v>0</v>
       </c>
       <c r="H204" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="205" spans="1:9">
@@ -3799,7 +3799,7 @@
         <v>158</v>
       </c>
       <c r="H205" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="I205" t="n">
         <v>1</v>
@@ -3830,7 +3830,7 @@
         <v>0</v>
       </c>
       <c r="H207" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="208" spans="1:9">
@@ -3841,7 +3841,7 @@
         <v>159</v>
       </c>
       <c r="H208" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I208" t="n">
         <v>1</v>
@@ -3872,7 +3872,7 @@
         <v>0</v>
       </c>
       <c r="H210" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="211" spans="1:9">
@@ -3883,7 +3883,7 @@
         <v>148</v>
       </c>
       <c r="H211" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I211" t="n">
         <v>1</v>
@@ -3922,7 +3922,7 @@
         <v>0</v>
       </c>
       <c r="H214" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="215" spans="1:9">
@@ -3933,7 +3933,7 @@
         <v>160</v>
       </c>
       <c r="H215" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I215" t="n">
         <v>1</v>
@@ -3947,7 +3947,7 @@
         <v>161</v>
       </c>
       <c r="H216" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="I216" t="n">
         <v>1</v>
@@ -4008,7 +4008,7 @@
         <v>0</v>
       </c>
       <c r="H221" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="222" spans="1:9">
@@ -4019,7 +4019,7 @@
         <v>137</v>
       </c>
       <c r="H222" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I222" t="n">
         <v>1</v>
@@ -4078,7 +4078,7 @@
         <v>0</v>
       </c>
       <c r="H226" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="227" spans="1:9">
@@ -4089,7 +4089,7 @@
         <v>158</v>
       </c>
       <c r="H227" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="I227" t="n">
         <v>1</v>
@@ -4120,7 +4120,7 @@
         <v>0</v>
       </c>
       <c r="H229" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="230" spans="1:9">
@@ -4131,7 +4131,7 @@
         <v>159</v>
       </c>
       <c r="H230" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I230" t="n">
         <v>1</v>
@@ -4162,7 +4162,7 @@
         <v>0</v>
       </c>
       <c r="H232" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="233" spans="1:9">
@@ -4173,7 +4173,7 @@
         <v>148</v>
       </c>
       <c r="H233" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I233" t="n">
         <v>1</v>
@@ -4212,7 +4212,7 @@
         <v>0</v>
       </c>
       <c r="H236" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="237" spans="1:9">
@@ -4223,7 +4223,7 @@
         <v>160</v>
       </c>
       <c r="H237" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I237" t="n">
         <v>1</v>
@@ -4237,7 +4237,7 @@
         <v>161</v>
       </c>
       <c r="H238" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="I238" t="n">
         <v>1</v>
@@ -4387,7 +4387,7 @@
         <v>167</v>
       </c>
       <c r="H250" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I250" t="n">
         <v>1</v>
@@ -4401,7 +4401,7 @@
         <v>168</v>
       </c>
       <c r="H251" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I251" t="n">
         <v>1</v>
@@ -4471,7 +4471,7 @@
         <v>172</v>
       </c>
       <c r="H256" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="I256" t="n">
         <v>1</v>
@@ -4720,7 +4720,7 @@
         <v>0</v>
       </c>
       <c r="H274" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="275" spans="1:9">
@@ -4731,7 +4731,7 @@
         <v>175</v>
       </c>
       <c r="H275" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I275" t="n">
         <v>1</v>
@@ -4745,7 +4745,7 @@
         <v>187</v>
       </c>
       <c r="H276" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="I276" t="n">
         <v>1</v>
@@ -4776,7 +4776,7 @@
         <v>0</v>
       </c>
       <c r="H278" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="279" spans="1:9">
@@ -4787,7 +4787,7 @@
         <v>190</v>
       </c>
       <c r="H279" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I279" t="n">
         <v>1</v>
@@ -4801,7 +4801,7 @@
         <v>191</v>
       </c>
       <c r="H280" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="I280" t="n">
         <v>1</v>
@@ -4865,7 +4865,7 @@
         <v>194</v>
       </c>
       <c r="H285" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I285" t="n">
         <v>1</v>
@@ -5105,7 +5105,7 @@
         <v>201</v>
       </c>
       <c r="H303" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I303" t="n">
         <v>1</v>
@@ -5283,7 +5283,7 @@
         <v>213</v>
       </c>
       <c r="H317" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I317" t="n">
         <v>1</v>
@@ -5339,7 +5339,7 @@
         <v>216</v>
       </c>
       <c r="H321" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I321" t="n">
         <v>1</v>
@@ -5436,7 +5436,7 @@
         <v>0</v>
       </c>
       <c r="H329" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="330" spans="1:9">
@@ -5447,7 +5447,7 @@
         <v>28</v>
       </c>
       <c r="H330" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="I330" t="n">
         <v>1</v>
@@ -5461,7 +5461,7 @@
         <v>29</v>
       </c>
       <c r="H331" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I331" t="n">
         <v>1</v>
@@ -5506,7 +5506,7 @@
         <v>0</v>
       </c>
       <c r="H334" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="335" spans="1:9">
@@ -5517,7 +5517,7 @@
         <v>33</v>
       </c>
       <c r="H335" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="I335" t="n">
         <v>1</v>
@@ -5531,7 +5531,7 @@
         <v>34</v>
       </c>
       <c r="H336" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I336" t="n">
         <v>1</v>
@@ -5562,7 +5562,7 @@
         <v>0</v>
       </c>
       <c r="H338" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="339" spans="1:9">
@@ -5573,7 +5573,7 @@
         <v>37</v>
       </c>
       <c r="H339" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="I339" t="n">
         <v>1</v>
@@ -5587,7 +5587,7 @@
         <v>38</v>
       </c>
       <c r="H340" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I340" t="n">
         <v>1</v>
@@ -5601,7 +5601,7 @@
         <v>39</v>
       </c>
       <c r="H341" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I341" t="n">
         <v>1</v>
@@ -5640,7 +5640,7 @@
         <v>0</v>
       </c>
       <c r="H344" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="345" spans="1:9">
@@ -5651,7 +5651,7 @@
         <v>43</v>
       </c>
       <c r="H345" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I345" t="n">
         <v>1</v>
@@ -5665,7 +5665,7 @@
         <v>44</v>
       </c>
       <c r="H346" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I346" t="n">
         <v>1</v>
@@ -5696,7 +5696,7 @@
         <v>0</v>
       </c>
       <c r="H348" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="349" spans="1:9">
@@ -5707,7 +5707,7 @@
         <v>223</v>
       </c>
       <c r="H349" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I349" t="n">
         <v>1</v>
@@ -5721,7 +5721,7 @@
         <v>224</v>
       </c>
       <c r="H350" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I350" t="n">
         <v>1</v>
@@ -5735,7 +5735,7 @@
         <v>225</v>
       </c>
       <c r="H351" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="I351" t="n">
         <v>1</v>
@@ -5805,7 +5805,7 @@
         <v>229</v>
       </c>
       <c r="H356" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I356" t="n">
         <v>1</v>
@@ -5819,7 +5819,7 @@
         <v>49</v>
       </c>
       <c r="H357" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I357" t="n">
         <v>1</v>
@@ -5875,7 +5875,7 @@
         <v>232</v>
       </c>
       <c r="H361" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I361" t="n">
         <v>1</v>
@@ -5889,7 +5889,7 @@
         <v>49</v>
       </c>
       <c r="H362" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I362" t="n">
         <v>1</v>
@@ -5945,7 +5945,7 @@
         <v>62</v>
       </c>
       <c r="H366" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I366" t="n">
         <v>1</v>
@@ -6009,7 +6009,7 @@
         <v>233</v>
       </c>
       <c r="H371" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I371" t="n">
         <v>1</v>
@@ -6056,7 +6056,7 @@
         <v>0</v>
       </c>
       <c r="H375" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="376" spans="1:9">
@@ -6067,7 +6067,7 @@
         <v>71</v>
       </c>
       <c r="H376" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="I376" t="n">
         <v>1</v>
@@ -6168,7 +6168,7 @@
         <v>0</v>
       </c>
       <c r="H383" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="384" spans="1:9">
@@ -6179,7 +6179,7 @@
         <v>80</v>
       </c>
       <c r="H384" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="I384" t="n">
         <v>1</v>
@@ -6193,7 +6193,7 @@
         <v>234</v>
       </c>
       <c r="H385" t="n">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="I385" t="n">
         <v>1</v>
@@ -6293,7 +6293,7 @@
         <v>239</v>
       </c>
       <c r="H393" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I393" t="n">
         <v>1</v>
@@ -6332,7 +6332,7 @@
         <v>0</v>
       </c>
       <c r="H396" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="397" spans="1:9">
@@ -6343,7 +6343,7 @@
         <v>243</v>
       </c>
       <c r="H397" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I397" t="n">
         <v>1</v>
@@ -6374,7 +6374,7 @@
         <v>0</v>
       </c>
       <c r="H399" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="400" spans="1:9">
@@ -6385,7 +6385,7 @@
         <v>246</v>
       </c>
       <c r="H400" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I400" t="n">
         <v>1</v>
@@ -6441,7 +6441,7 @@
         <v>250</v>
       </c>
       <c r="H404" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I404" t="n">
         <v>1</v>
@@ -6497,7 +6497,7 @@
         <v>254</v>
       </c>
       <c r="H408" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I408" t="n">
         <v>1</v>
@@ -6567,7 +6567,7 @@
         <v>258</v>
       </c>
       <c r="H413" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I413" t="n">
         <v>1</v>
@@ -6614,7 +6614,7 @@
         <v>0</v>
       </c>
       <c r="H417" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="418" spans="1:9">
@@ -6625,7 +6625,7 @@
         <v>71</v>
       </c>
       <c r="H418" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="I418" t="n">
         <v>1</v>
@@ -6726,7 +6726,7 @@
         <v>0</v>
       </c>
       <c r="H425" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="426" spans="1:9">
@@ -6737,7 +6737,7 @@
         <v>80</v>
       </c>
       <c r="H426" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="I426" t="n">
         <v>1</v>

</xml_diff>